<commit_message>
Agenda nog iets aangepast
</commit_message>
<xml_diff>
--- a/Agenda en Notulen/Agenda week 1.xlsx
+++ b/Agenda en Notulen/Agenda week 1.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>wie</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Agenda aan:  Alle betrokkenen</t>
+  </si>
+  <si>
+    <t>Aftekenlijst van project</t>
   </si>
 </sst>
 </file>
@@ -909,7 +912,9 @@
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1324,7 +1329,9 @@
       <c r="E34" s="4">
         <v>1</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="I34" s="49"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
@@ -1460,9 +1467,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1515,24 +1525,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1553,9 +1554,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>